<commit_message>
added some new files to play with complete_structures function
</commit_message>
<xml_diff>
--- a/SP500-regression-nodates.xlsx
+++ b/SP500-regression-nodates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xaos\Desktop\General Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21331867-7FF1-4D0E-B92D-76E85F2D1FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CC563F-E0D9-4588-89A9-7309DC23197C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1809"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
deleted useless files and added some new ones
</commit_message>
<xml_diff>
--- a/SP500-regression-nodates.xlsx
+++ b/SP500-regression-nodates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xaos\Desktop\General Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CC563F-E0D9-4588-89A9-7309DC23197C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8C6BE1-B6E7-47A7-BF88-0CF3421EEE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1809"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>